<commit_message>
Revert "Actualizando normalizacion cliente"
This reverts commit 117ef0df748de5d68de5749d07c1fdab17d4b066.
</commit_message>
<xml_diff>
--- a/base de datos normalizada.xlsx
+++ b/base de datos normalizada.xlsx
@@ -4,14 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" tabRatio="670" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" tabRatio="670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="relaciones" sheetId="1" r:id="rId1"/>
     <sheet name="formalizacion 3 formas" sheetId="6" r:id="rId2"/>
     <sheet name="Clientes" sheetId="7" r:id="rId3"/>
-    <sheet name="Cliente" sheetId="8" r:id="rId4"/>
-    <sheet name="Configuraciones" sheetId="9" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -322,7 +320,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="212">
   <si>
     <t>id</t>
   </si>
@@ -958,186 +956,6 @@
   </si>
   <si>
     <t>GeneroID</t>
-  </si>
-  <si>
-    <t>ClienteID</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Nacimiento</t>
-  </si>
-  <si>
-    <t>Ocupacion</t>
-  </si>
-  <si>
-    <t>Telefono</t>
-  </si>
-  <si>
-    <t>Direccion</t>
-  </si>
-  <si>
-    <t>Sueldo</t>
-  </si>
-  <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
-    <t>Claro dominincana</t>
-  </si>
-  <si>
-    <t>Programador</t>
-  </si>
-  <si>
-    <t>Tiempo</t>
-  </si>
-  <si>
-    <t>5 años</t>
-  </si>
-  <si>
-    <t>Celular</t>
-  </si>
-  <si>
-    <t>Documento</t>
-  </si>
-  <si>
-    <t>01201103502</t>
-  </si>
-  <si>
-    <t>10/08/1990</t>
-  </si>
-  <si>
-    <t>Dependiente</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Correo</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>8496364367</t>
-  </si>
-  <si>
-    <t>UsuarioID</t>
-  </si>
-  <si>
-    <t>Estado_Civil</t>
-  </si>
-  <si>
-    <t>Soltero</t>
-  </si>
-  <si>
-    <t>Rosa</t>
-  </si>
-  <si>
-    <t>NacionalidadID</t>
-  </si>
-  <si>
-    <t>EmpresaID</t>
-  </si>
-  <si>
-    <t>Credifassil</t>
-  </si>
-  <si>
-    <t>Estado</t>
-  </si>
-  <si>
-    <t>Cliente_Conyuge</t>
-  </si>
-  <si>
-    <t>Cliente_Empleo</t>
-  </si>
-  <si>
-    <t>Rosalis perez</t>
-  </si>
-  <si>
-    <t>8298922597</t>
-  </si>
-  <si>
-    <t>Cliente_Referencia</t>
-  </si>
-  <si>
-    <t>Juan carlos</t>
-  </si>
-  <si>
-    <t>8296365487</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Carlos gomez</t>
-  </si>
-  <si>
-    <t>8496258745</t>
-  </si>
-  <si>
-    <t>Jeuris hernandez</t>
-  </si>
-  <si>
-    <t>8296578457</t>
-  </si>
-  <si>
-    <t>Cliente_Otros</t>
-  </si>
-  <si>
-    <t>Detalle</t>
-  </si>
-  <si>
-    <t>facebook: adel sanchez</t>
-  </si>
-  <si>
-    <t>Correo personal: adelsanchez67@yahoo.es</t>
-  </si>
-  <si>
-    <t>Casado</t>
-  </si>
-  <si>
-    <t>Union libre</t>
-  </si>
-  <si>
-    <t>Dominicana</t>
-  </si>
-  <si>
-    <t>Haitiana</t>
-  </si>
-  <si>
-    <t>Cubana</t>
-  </si>
-  <si>
-    <t>Venezolana</t>
-  </si>
-  <si>
-    <t>calle beltram 36</t>
-  </si>
-  <si>
-    <t>credifassil@hotmail.com</t>
-  </si>
-  <si>
-    <t>Facebook</t>
-  </si>
-  <si>
-    <t>Rnc</t>
-  </si>
-  <si>
-    <t>Empresa_Otros</t>
-  </si>
-  <si>
-    <t>Registro:152458445</t>
-  </si>
-  <si>
-    <t>Clave</t>
-  </si>
-  <si>
-    <t>Marlyn Miraval</t>
-  </si>
-  <si>
-    <t>marlin@credifassil.com.do</t>
   </si>
 </sst>
 </file>
@@ -1198,7 +1016,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1241,36 +1059,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1299,7 +1087,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1406,85 +1194,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1757,7 +1466,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2583,8 +2292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AJ68"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:F54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4634,685 +4343,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:O32"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.5703125" style="40" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="40" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" style="40" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" style="40" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="40" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="40" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="40" customWidth="1"/>
-    <col min="8" max="8" width="12" style="40" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" style="40" customWidth="1"/>
-    <col min="10" max="10" width="12.5703125" style="40" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" style="40" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="40"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>213</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>214</v>
-      </c>
-      <c r="D3" s="45" t="s">
-        <v>225</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>228</v>
-      </c>
-      <c r="F3" s="45" t="s">
-        <v>224</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="I3" s="50" t="s">
-        <v>237</v>
-      </c>
-      <c r="J3" s="45" t="s">
-        <v>238</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>233</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>240</v>
-      </c>
-      <c r="M3"/>
-      <c r="N3"/>
-      <c r="O3"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="46">
-        <v>1</v>
-      </c>
-      <c r="B4" s="46" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="51" t="s">
-        <v>227</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>226</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>229</v>
-      </c>
-      <c r="F4" s="46" t="s">
-        <v>232</v>
-      </c>
-      <c r="G4" s="46" t="s">
-        <v>235</v>
-      </c>
-      <c r="H4" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="I4" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="46" t="s">
-        <v>239</v>
-      </c>
-      <c r="K4" s="46" t="s">
-        <v>236</v>
-      </c>
-      <c r="L4" s="46" t="s">
-        <v>231</v>
-      </c>
-      <c r="M4"/>
-      <c r="N4"/>
-      <c r="O4"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
-        <v>242</v>
-      </c>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="42"/>
-      <c r="H7"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
-        <v>213</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>212</v>
-      </c>
-      <c r="C8" s="41" t="s">
-        <v>147</v>
-      </c>
-      <c r="D8" s="41" t="s">
-        <v>215</v>
-      </c>
-      <c r="E8" s="41" t="s">
-        <v>216</v>
-      </c>
-      <c r="F8" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>222</v>
-      </c>
-      <c r="H8"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="42">
-        <v>1</v>
-      </c>
-      <c r="B9" s="42" t="s">
-        <v>231</v>
-      </c>
-      <c r="C9" s="42" t="s">
-        <v>220</v>
-      </c>
-      <c r="D9" s="42" t="s">
-        <v>221</v>
-      </c>
-      <c r="E9" s="42">
-        <v>8092208217</v>
-      </c>
-      <c r="F9" s="42">
-        <v>55000</v>
-      </c>
-      <c r="G9" s="42" t="s">
-        <v>223</v>
-      </c>
-      <c r="H9"/>
-      <c r="I9" s="47"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="42"/>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
-        <v>241</v>
-      </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="47"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
-        <v>213</v>
-      </c>
-      <c r="B15" s="43" t="s">
-        <v>212</v>
-      </c>
-      <c r="C15" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="D15" s="43" t="s">
-        <v>224</v>
-      </c>
-      <c r="E15" s="47"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="47"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="B16" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="C16" s="44" t="s">
-        <v>243</v>
-      </c>
-      <c r="D16" s="44" t="s">
-        <v>244</v>
-      </c>
-      <c r="E16" s="47"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="47"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="44"/>
-      <c r="B17" s="43"/>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="s">
-        <v>245</v>
-      </c>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="B22" s="49" t="s">
-        <v>212</v>
-      </c>
-      <c r="C22" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="D22" s="49" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="48" t="s">
-        <v>231</v>
-      </c>
-      <c r="B23" s="48" t="s">
-        <v>231</v>
-      </c>
-      <c r="C23" s="48" t="s">
-        <v>246</v>
-      </c>
-      <c r="D23" s="48" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="48" t="s">
-        <v>248</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>231</v>
-      </c>
-      <c r="C24" s="48" t="s">
-        <v>249</v>
-      </c>
-      <c r="D24" s="48" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="48" t="s">
-        <v>229</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>231</v>
-      </c>
-      <c r="C25" s="48" t="s">
-        <v>251</v>
-      </c>
-      <c r="D25" s="48" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
-        <v>253</v>
-      </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="54"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="53" t="s">
-        <v>213</v>
-      </c>
-      <c r="B29" s="53" t="s">
-        <v>212</v>
-      </c>
-      <c r="C29" s="53" t="s">
-        <v>254</v>
-      </c>
-      <c r="D29" s="54"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="B30" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="C30" s="54" t="s">
-        <v>255</v>
-      </c>
-      <c r="D30" s="54"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
-        <v>248</v>
-      </c>
-      <c r="B31" s="54" t="s">
-        <v>231</v>
-      </c>
-      <c r="C31" s="54" t="s">
-        <v>256</v>
-      </c>
-      <c r="D31" s="54"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="54"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G39"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="18" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" style="18" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="18" customWidth="1"/>
-    <col min="5" max="5" width="23" style="18" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="18" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="18" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="18" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="18"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
-        <v>234</v>
-      </c>
-      <c r="B2" s="56"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="55" t="s">
-        <v>213</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="56">
-        <v>1</v>
-      </c>
-      <c r="B4" s="56" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="56">
-        <v>2</v>
-      </c>
-      <c r="B5" s="56" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="56">
-        <v>3</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
-        <v>210</v>
-      </c>
-      <c r="B9" s="59"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="B10" s="59" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="60">
-        <v>1</v>
-      </c>
-      <c r="B11" s="60" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="60">
-        <v>2</v>
-      </c>
-      <c r="B12" s="60" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="57" t="s">
-        <v>183</v>
-      </c>
-      <c r="B16" s="57"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="57" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17" s="57" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="58">
-        <v>1</v>
-      </c>
-      <c r="B18" s="58" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="58">
-        <v>2</v>
-      </c>
-      <c r="B19" s="58" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="58">
-        <v>3</v>
-      </c>
-      <c r="B20" s="58" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="58">
-        <v>4</v>
-      </c>
-      <c r="B21" s="58" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="61" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="61" t="s">
-        <v>213</v>
-      </c>
-      <c r="B25" s="61" t="s">
-        <v>147</v>
-      </c>
-      <c r="C25" s="61" t="s">
-        <v>217</v>
-      </c>
-      <c r="D25" s="61" t="s">
-        <v>216</v>
-      </c>
-      <c r="E25" s="61" t="s">
-        <v>230</v>
-      </c>
-      <c r="F25" s="61" t="s">
-        <v>265</v>
-      </c>
-      <c r="G25" s="61" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="62">
-        <v>1</v>
-      </c>
-      <c r="B26" s="62" t="s">
-        <v>239</v>
-      </c>
-      <c r="C26" s="62" t="s">
-        <v>263</v>
-      </c>
-      <c r="D26" s="62">
-        <v>8096351254</v>
-      </c>
-      <c r="E26" s="63" t="s">
-        <v>264</v>
-      </c>
-      <c r="F26" s="62" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="62">
-        <v>8526587558</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="62"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="66" t="s">
-        <v>267</v>
-      </c>
-      <c r="B30" s="66"/>
-      <c r="C30" s="66"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="66" t="s">
-        <v>213</v>
-      </c>
-      <c r="B31" s="66" t="s">
-        <v>238</v>
-      </c>
-      <c r="C31" s="66" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="67">
-        <v>1</v>
-      </c>
-      <c r="B32" s="67">
-        <v>1</v>
-      </c>
-      <c r="C32" s="67" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="67"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="64" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="64"/>
-      <c r="C36" s="64"/>
-      <c r="D36" s="64"/>
-      <c r="E36" s="64"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="64" t="s">
-        <v>213</v>
-      </c>
-      <c r="B37" s="64" t="s">
-        <v>238</v>
-      </c>
-      <c r="C37" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="D37" s="64" t="s">
-        <v>230</v>
-      </c>
-      <c r="E37" s="64" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="65">
-        <v>1</v>
-      </c>
-      <c r="B38" s="65">
-        <v>1</v>
-      </c>
-      <c r="C38" s="65" t="s">
-        <v>270</v>
-      </c>
-      <c r="D38" s="68" t="s">
-        <v>271</v>
-      </c>
-      <c r="E38" s="65">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="65"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="65"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="65"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
agregue pagina de net core 2.2
</commit_message>
<xml_diff>
--- a/base de datos normalizada.xlsx
+++ b/base de datos normalizada.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" tabRatio="670" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7080" tabRatio="670" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="relaciones" sheetId="1" r:id="rId1"/>
@@ -326,7 +326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="150">
   <si>
     <t>id</t>
   </si>
@@ -773,6 +773,9 @@
   </si>
   <si>
     <t>credifassil.com.do</t>
+  </si>
+  <si>
+    <t>20000</t>
   </si>
 </sst>
 </file>
@@ -1061,14 +1064,14 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1370,12 +1373,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
     </row>
@@ -1416,12 +1419,12 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="50"/>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -1525,11 +1528,11 @@
       <c r="A17"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="50"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
     </row>
     <row r="19" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -2168,8 +2171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,8 +2351,8 @@
       <c r="F9" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="G9" s="25">
-        <v>55000</v>
+      <c r="G9" s="25" t="s">
+        <v>149</v>
       </c>
       <c r="H9" s="25" t="s">
         <v>92</v>
@@ -2375,46 +2378,46 @@
       <c r="A12" s="30"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="51" t="s">
+      <c r="A14" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="50" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="52" t="s">
+      <c r="A15" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="51" t="s">
         <v>100</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="51" t="s">
         <v>142</v>
       </c>
-      <c r="D15" s="52" t="s">
+      <c r="D15" s="51" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="52"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="30"/>
@@ -2611,7 +2614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>

</xml_diff>